<commit_message>
add initial calculations for heat sync
</commit_message>
<xml_diff>
--- a/mppt/design/Converter_calculations.xlsx
+++ b/mppt/design/Converter_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD83118-037C-4BA8-B5E2-D914471F614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F642484-77B3-4495-B43F-A32EFA225EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId1"/>
@@ -40,6 +40,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows PC</author>
+    <author>Shelby Riggleman</author>
   </authors>
   <commentList>
     <comment ref="E7" authorId="0" shapeId="0" xr:uid="{C4638315-B48B-48DE-A9B9-BE8E74762BF5}">
@@ -54,6 +55,31 @@
           </rPr>
           <t>S. Riggleman:
 For 8 bit PWM Resolution, fPWM = ~280kHz</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB7" authorId="1" shapeId="0" xr:uid="{6ADE8147-1C8E-4C60-8ED7-B9B2F96D6B65}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby Riggleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Resource here:
+https://www.cuidevices.com/blog/how-to-select-a-heat-sink</t>
         </r>
       </text>
     </comment>
@@ -449,7 +475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="154">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -863,6 +889,54 @@
   </si>
   <si>
     <t>Power Consumed</t>
+  </si>
+  <si>
+    <t>Thermal coefficient JA (C/W):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heatsink </t>
+  </si>
+  <si>
+    <t>Max Ambient Temp C:</t>
+  </si>
+  <si>
+    <t>Target Max FET Junction Temp C:</t>
+  </si>
+  <si>
+    <t>Maximum Junction Temp C:</t>
+  </si>
+  <si>
+    <t>Permissible J/A temp diff:</t>
+  </si>
+  <si>
+    <t>FET Power Dissipation (W):</t>
+  </si>
+  <si>
+    <t>Largest Permissible thermal impedance:</t>
+  </si>
+  <si>
+    <t>Thermal coefficient JC (C/W):</t>
+  </si>
+  <si>
+    <t>TIM Parameters:</t>
+  </si>
+  <si>
+    <t>Thermal conductivity (W/MC):</t>
+  </si>
+  <si>
+    <t>Area of application (M^2)</t>
+  </si>
+  <si>
+    <t>Thickness of application (M)</t>
+  </si>
+  <si>
+    <t>Thermal Resistance Case/Sink (C/W):</t>
+  </si>
+  <si>
+    <t>Resultant Values:</t>
+  </si>
+  <si>
+    <t>Max heatsink Resistance Sink/Ambient (C/W)</t>
   </si>
 </sst>
 </file>
@@ -984,13 +1058,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1777,48 +1851,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="41.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="G1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1829,11 +1904,11 @@
         <v>67</v>
       </c>
       <c r="H3">
-        <f>SUM(K31,K29,K27,K25,H26,H24,N23,Y23)</f>
+        <f>SUM(K34,K32,K30,K28,H26,H24,N23,Y23)</f>
         <v>25.043733816358454</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -1842,27 +1917,27 @@
         <v>0.97144255859291362</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1895,11 +1970,14 @@
         <v>101</v>
       </c>
       <c r="V7" s="11"/>
-      <c r="X7" t="s">
+      <c r="X7" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB7" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1953,8 +2031,14 @@
       <c r="Y8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1993,8 +2077,14 @@
       <c r="Y9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2027,8 +2117,15 @@
       <c r="Y10">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC10">
+        <f>AC9-AC8</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -2041,8 +2138,15 @@
       <c r="N11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC11">
+        <f>K26+K29+K31+K33</f>
+        <v>5.3462160000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2053,8 +2157,15 @@
         <f>E11*B19</f>
         <v>833.11199999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB12" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC12">
+        <f>AC10/AC11</f>
+        <v>15.89909573425391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2089,7 +2200,7 @@
       </c>
       <c r="V13" s="11"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -2124,8 +2235,11 @@
       <c r="V14" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB14" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2155,8 +2269,14 @@
         <f>1000*POWER(10,-6)</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB15" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC15">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2183,8 +2303,14 @@
       <c r="V16">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC16">
+        <v>1.12E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2211,8 +2337,14 @@
       <c r="V17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC17">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2233,8 +2365,15 @@
       <c r="V18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB18" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC18">
+        <f>(AC17/AC16)*(1/AC15)</f>
+        <v>0.4520795660036166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2254,7 +2393,7 @@
         <v>4.7800000000000002E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G20" s="5" t="s">
         <v>34</v>
       </c>
@@ -2270,7 +2409,7 @@
         <v>1.8666666666666668E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G21" s="5" t="s">
         <v>35</v>
       </c>
@@ -2278,8 +2417,17 @@
         <f>E13+(0.5*H20)</f>
         <v>7.4996625000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="J21" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21">
+        <v>62</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2287,10 +2435,12 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>6.0621499930279485</v>
       </c>
-      <c r="J22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="11"/>
+      <c r="J22" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22">
+        <v>0.5</v>
+      </c>
       <c r="M22" s="10" t="s">
         <v>33</v>
       </c>
@@ -2303,8 +2453,15 @@
         <v>33</v>
       </c>
       <c r="Y22" s="11"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB22" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC22">
+        <f>AC12-AC18-K22</f>
+        <v>14.947016168250293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G23" s="5" t="s">
         <v>36</v>
       </c>
@@ -2313,11 +2470,10 @@
         <v>0.84156727211948457</v>
       </c>
       <c r="J23" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="K23">
-        <f>POWER(K8,2)*K15</f>
-        <v>0.12765599999999996</v>
+        <v>175</v>
       </c>
       <c r="M23" t="s">
         <v>97</v>
@@ -2341,7 +2497,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G24" s="5" t="s">
         <v>37</v>
       </c>
@@ -2349,13 +2505,6 @@
         <f>H23*B8</f>
         <v>2.5247018163584536</v>
       </c>
-      <c r="J24" t="s">
-        <v>44</v>
-      </c>
-      <c r="K24">
-        <f>POWER(K9,2)*K15</f>
-        <v>0.13154400000000005</v>
-      </c>
       <c r="M24" t="s">
         <v>98</v>
       </c>
@@ -2371,20 +2520,17 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H25">
         <v>1.78E-2</v>
       </c>
-      <c r="J25" t="s">
-        <v>43</v>
-      </c>
-      <c r="K25">
-        <f>SUM(K23:K24)*B8</f>
-        <v>0.77759999999999996</v>
-      </c>
+      <c r="J25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="11"/>
       <c r="U25" t="s">
         <v>108</v>
       </c>
@@ -2393,7 +2539,7 @@
         <v>9.2322972656249998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G26" s="5" t="s">
         <v>53</v>
       </c>
@@ -2402,11 +2548,11 @@
         <v>5.3400000000000003E-2</v>
       </c>
       <c r="J26" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="K26">
-        <f>B18*E13*K20*E8</f>
-        <v>0.86016000000000015</v>
+        <f>POWER(K8,2)*K15</f>
+        <v>0.12765599999999996</v>
       </c>
       <c r="U26" t="s">
         <v>110</v>
@@ -2416,13 +2562,13 @@
         <v>5.6999999999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K27">
-        <f>K26*B8</f>
-        <v>2.5804800000000006</v>
+        <f>POWER(K9,2)*K15</f>
+        <v>0.13154400000000005</v>
       </c>
       <c r="U27" t="s">
         <v>111</v>
@@ -2432,13 +2578,13 @@
         <v>0.11399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="K28">
-        <f>(K18/2)*B18*E8</f>
-        <v>0.68735999999999997</v>
+        <f>SUM(K26:K27)*B8</f>
+        <v>0.77759999999999996</v>
       </c>
       <c r="U28" t="s">
         <v>112</v>
@@ -2448,35 +2594,65 @@
         <v>0.11437322812966706</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29">
+        <f>B18*E13*K20*E8</f>
+        <v>0.86016000000000015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30">
+        <f>K29*B8</f>
+        <v>2.5804800000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K31">
+        <f>(K18/2)*B18*E8</f>
+        <v>0.68735999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
         <v>60</v>
       </c>
-      <c r="K29">
-        <f>K28*2*B8</f>
+      <c r="K32">
+        <f>K31*2*B8</f>
         <v>4.1241599999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="J30" t="s">
+    <row r="33" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
         <v>64</v>
       </c>
-      <c r="K30">
+      <c r="K33">
         <f>K19*B18*E8</f>
         <v>3.6710400000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="J31" t="s">
+    <row r="34" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
         <v>65</v>
       </c>
-      <c r="K31">
-        <f>K30*B8</f>
+      <c r="K34">
+        <f>K33*B8</f>
         <v>11.013120000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="X22:Y22"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
@@ -2486,16 +2662,13 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J25:K25"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U22:V22"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -2518,16 +2691,16 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -2535,7 +2708,7 @@
         <v>74437529203101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2543,7 +2716,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -2551,7 +2724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -2559,7 +2732,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -2567,7 +2740,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2575,7 +2748,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2583,7 +2756,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2591,7 +2764,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>128</v>
       </c>
@@ -2601,7 +2774,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -2611,7 +2784,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -2621,12 +2794,12 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2660,40 +2833,40 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="G1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2708,7 +2881,7 @@
         <v>40.475782132134938</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -2717,27 +2890,27 @@
         <v>0.95384534969424506</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2763,7 +2936,7 @@
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2798,7 +2971,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2832,7 +3005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2860,7 +3033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -2874,7 +3047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2886,7 +3059,7 @@
         <v>833.11199999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2913,7 +3086,7 @@
       </c>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -2940,7 +3113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2964,7 +3137,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2986,7 +3159,7 @@
         <v>7.0000000000000005E-8</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3008,7 +3181,7 @@
         <v>5.6000000000000005E-8</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3024,7 +3197,7 @@
         <v>1.79E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3044,7 +3217,7 @@
         <v>4.7800000000000002E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G20" s="5" t="s">
         <v>34</v>
       </c>
@@ -3060,7 +3233,7 @@
         <v>1.8666666666666668E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G21" s="5" t="s">
         <v>35</v>
       </c>
@@ -3069,7 +3242,7 @@
         <v>11.423696969696969</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
@@ -3086,7 +3259,7 @@
       </c>
       <c r="N22" s="10"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G23" s="5" t="s">
         <v>36</v>
       </c>
@@ -3109,7 +3282,7 @@
         <v>1.63212</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G24" s="5" t="s">
         <v>37</v>
       </c>
@@ -3132,7 +3305,7 @@
         <v>4.8963599999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
         <v>52</v>
       </c>
@@ -3147,7 +3320,7 @@
         <v>1.1663999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G26" s="5" t="s">
         <v>53</v>
       </c>
@@ -3163,7 +3336,7 @@
         <v>3.6288000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
         <v>46</v>
       </c>
@@ -3172,7 +3345,7 @@
         <v>7.2576000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>62</v>
       </c>
@@ -3181,7 +3354,7 @@
         <v>1.9332</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>60</v>
       </c>
@@ -3190,7 +3363,7 @@
         <v>7.7328000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J30" t="s">
         <v>64</v>
       </c>
@@ -3199,7 +3372,7 @@
         <v>10.324800000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J31" t="s">
         <v>65</v>
       </c>
@@ -3210,6 +3383,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:N5"/>
@@ -3217,12 +3396,6 @@
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
@@ -3244,14 +3417,14 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -3274,7 +3447,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -3298,7 +3471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -3316,7 +3489,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -3327,7 +3500,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -3348,7 +3521,7 @@
         <v>1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
initial placement on power stage
</commit_message>
<xml_diff>
--- a/mppt/design/Converter_calculations.xlsx
+++ b/mppt/design/Converter_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42AA5CC-46BA-4A38-9DE2-E3BDDE5C64EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC74F79E-FFFA-43F8-9D5F-A5BD5CA5AB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="165">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -843,9 +843,6 @@
     <t>UCY2G101MHD6</t>
   </si>
   <si>
-    <t>1.75 @ 100hz</t>
-  </si>
-  <si>
     <t>Power Inductor:</t>
   </si>
   <si>
@@ -979,6 +976,24 @@
   </si>
   <si>
     <t>Rule of thumb 33% increase thermal resistance for point load thermal connection:</t>
+  </si>
+  <si>
+    <t>1.75 @ 100khz</t>
+  </si>
+  <si>
+    <t>Transitioned to multi string single phase design on different sheet. Primary reason was too high of switching losses at switching frequency needed to keep inductor in CCM. Higher inductance values could fix this by moving to  lesser frequency (which is what we do on new design), but parts with  inductance values with &gt; 9A sat current are few, and we want options in supply shortage. IN addition, having seperate MPPT's per string allows for most efficienct MPPT tracking and prevention of false mppt peaks when combining multiple strings together if one is shaded.</t>
+  </si>
+  <si>
+    <t>Open Questions:</t>
+  </si>
+  <si>
+    <t>Why does boost FET incur QRR losses and not sync fet?</t>
+  </si>
+  <si>
+    <t>How to assess stability of system (gain/phase margin)</t>
+  </si>
+  <si>
+    <t>CCM vs DCM mode of operation advantages?</t>
   </si>
 </sst>
 </file>
@@ -1094,11 +1109,8 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1106,14 +1118,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1899,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC36" sqref="AC36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1921,25 +1936,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1969,21 +1984,21 @@
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1995,34 +2010,34 @@
       <c r="E7">
         <v>80000</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="14"/>
+      <c r="J7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="10" t="s">
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="10"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="10"/>
-      <c r="U7" s="10" t="s">
+      <c r="S7" s="13"/>
+      <c r="U7" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="11"/>
+      <c r="V7" s="14"/>
       <c r="X7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -2074,13 +2089,13 @@
         <v>2.849679356962814</v>
       </c>
       <c r="X8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC8">
         <v>45</v>
@@ -2120,13 +2135,13 @@
         <v>69</v>
       </c>
       <c r="X9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Y9">
         <v>0.3</v>
       </c>
       <c r="AB9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC9">
         <v>125</v>
@@ -2166,7 +2181,7 @@
         <v>12</v>
       </c>
       <c r="AB10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC10">
         <f>AC9-AC8</f>
@@ -2187,7 +2202,7 @@
         <v>74</v>
       </c>
       <c r="AB11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC11">
         <f>K26+K29+K31+K33</f>
@@ -2206,7 +2221,7 @@
         <v>833.11199999999997</v>
       </c>
       <c r="AB12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC12">
         <f>AC10/AC11</f>
@@ -2227,26 +2242,26 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="J13" s="10" t="s">
+      <c r="H13" s="13"/>
+      <c r="J13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="M13" s="10" t="s">
+      <c r="K13" s="14"/>
+      <c r="M13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="R13" s="10" t="s">
+      <c r="N13" s="13"/>
+      <c r="R13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="10"/>
-      <c r="U13" s="10" t="s">
+      <c r="S13" s="13"/>
+      <c r="U13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="11"/>
+      <c r="V13" s="14"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -2284,7 +2299,7 @@
         <v>113</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
@@ -2318,7 +2333,7 @@
         <v>1E-3</v>
       </c>
       <c r="AB15" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC15">
         <v>0.79</v>
@@ -2352,7 +2367,7 @@
         <v>0.02</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AC16">
         <v>1.12E-4</v>
@@ -2383,10 +2398,10 @@
         <v>107</v>
       </c>
       <c r="V17" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="AB17" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC17">
         <v>4.0000000000000003E-5</v>
@@ -2411,10 +2426,10 @@
         <v>109</v>
       </c>
       <c r="V18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC18">
         <f>(AC17/AC16)*(1/AC15)</f>
@@ -2429,10 +2444,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="13"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2466,13 +2481,13 @@
         <v>7.4996625000000003</v>
       </c>
       <c r="J21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K21">
         <v>62</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
@@ -2484,25 +2499,25 @@
         <v>6.0621499930279485</v>
       </c>
       <c r="J22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K22">
         <v>0.5</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="M22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="U22" s="10" t="s">
+      <c r="N22" s="14"/>
+      <c r="U22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="X22" s="10" t="s">
+      <c r="V22" s="14"/>
+      <c r="X22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Y22" s="11"/>
+      <c r="Y22" s="14"/>
       <c r="AB22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AC22">
         <f>AC12-AC18-K22</f>
@@ -2518,7 +2533,7 @@
         <v>0.84156727211948457</v>
       </c>
       <c r="J23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K23">
         <v>175</v>
@@ -2535,19 +2550,19 @@
       </c>
       <c r="V23">
         <f>V18*V15</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="X23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y23">
         <f>Y10*Y9</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="AB23" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC23" s="11">
+        <v>153</v>
+      </c>
+      <c r="AC23" s="14">
         <f>AC22*0.666</f>
         <v>9.3318423116421592</v>
       </c>
@@ -2572,10 +2587,10 @@
       </c>
       <c r="V24">
         <f>V16/V18</f>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AB24" s="15"/>
-      <c r="AC24" s="11"/>
+      <c r="AC24" s="14"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
@@ -2584,19 +2599,19 @@
       <c r="H25">
         <v>1.78E-2</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="11"/>
+      <c r="K25" s="14"/>
       <c r="U25" t="s">
         <v>108</v>
       </c>
       <c r="V25">
         <f>(H20*E10)/(E8*V23)</f>
-        <v>9.2322972656249998E-3</v>
+        <v>1.846459453125E-2</v>
       </c>
       <c r="AB25" s="15"/>
-      <c r="AC25" s="11"/>
+      <c r="AC25" s="14"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G26" s="5" t="s">
@@ -2650,7 +2665,7 @@
       </c>
       <c r="V28">
         <f>SQRT(POWER(V25,2) + POWER(V27,2))</f>
-        <v>0.11437322812966706</v>
+        <v>0.11548567552386514</v>
       </c>
       <c r="AB28" s="1" t="s">
         <v>26</v>
@@ -2665,10 +2680,10 @@
         <v>0.86016000000000015</v>
       </c>
       <c r="AB29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC29" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="AC29" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
@@ -2680,7 +2695,7 @@
         <v>2.5804800000000006</v>
       </c>
       <c r="AB30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC30">
         <v>5.6</v>
@@ -2694,8 +2709,8 @@
         <f>(K18/2)*B18*E8</f>
         <v>0.68735999999999997</v>
       </c>
-      <c r="AB31" s="16" t="s">
-        <v>159</v>
+      <c r="AB31" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="AC31">
         <f>AC30*1.33</f>
@@ -2710,9 +2725,9 @@
         <f>K31*2*B8</f>
         <v>4.1241599999999998</v>
       </c>
-      <c r="AB32" s="16"/>
-    </row>
-    <row r="33" spans="10:29" x14ac:dyDescent="0.3">
+      <c r="AB32" s="10"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J33" t="s">
         <v>64</v>
       </c>
@@ -2721,7 +2736,7 @@
         <v>3.6710400000000005</v>
       </c>
     </row>
-    <row r="34" spans="10:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J34" t="s">
         <v>65</v>
       </c>
@@ -2733,13 +2748,31 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="10:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
       <c r="AB35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AC35">
         <f>AC11*(K22+AC18+AC31)+AC8</f>
         <v>89.908639777041586</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2757,14 +2790,14 @@
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -2799,7 +2832,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="7">
         <v>74437529203101</v>
@@ -2807,7 +2840,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>63</v>
@@ -2815,7 +2848,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>69</v>
@@ -2823,7 +2856,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>113</v>
@@ -2831,62 +2864,62 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2924,10 +2957,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2942,28 +2975,28 @@
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +3011,7 @@
         <v>40.475782132134938</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -2987,27 +3020,36 @@
         <v>0.95384534969424506</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3017,23 +3059,28 @@
       <c r="E7">
         <v>450000</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="14"/>
+      <c r="J7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11" t="s">
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3067,8 +3114,13 @@
       <c r="N8" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3101,8 +3153,13 @@
       <c r="N9" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3129,8 +3186,13 @@
       <c r="N10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -3143,8 +3205,13 @@
       <c r="N11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -3155,8 +3222,13 @@
         <f>E11*B19</f>
         <v>833.11199999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3170,20 +3242,25 @@
         <f>(B17/E9)</f>
         <v>9</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="J13" s="10" t="s">
+      <c r="H13" s="13"/>
+      <c r="J13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="M13" s="10" t="s">
+      <c r="K13" s="14"/>
+      <c r="M13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N13" s="13"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -3209,8 +3286,13 @@
       <c r="N14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3233,8 +3315,13 @@
       <c r="N15">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3255,6 +3342,11 @@
         <f>70*POWER(10,-9)</f>
         <v>7.0000000000000005E-8</v>
       </c>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -3302,10 +3394,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="13"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -3347,14 +3439,14 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="11"/>
-      <c r="M22" s="10" t="s">
+      <c r="K22" s="14"/>
+      <c r="M22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="10"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G23" s="5" t="s">
@@ -3479,7 +3571,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="R6:V16"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:N5"/>

</xml_diff>

<commit_message>
add calculations for diode rectifier
</commit_message>
<xml_diff>
--- a/mppt/design/Converter_calculations.xlsx
+++ b/mppt/design/Converter_calculations.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC74F79E-FFFA-43F8-9D5F-A5BD5CA5AB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4841EE-0056-4E05-8580-36FCDA5FF8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
-    <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId1"/>
-    <sheet name="Library_Parts_To_Make" sheetId="5" r:id="rId2"/>
-    <sheet name="Original_Multiphase" sheetId="1" r:id="rId3"/>
-    <sheet name="POL_Power_Breakdown" sheetId="4" r:id="rId4"/>
+    <sheet name="Multi_String_with_diode" sheetId="6" r:id="rId1"/>
+    <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId2"/>
+    <sheet name="Library_Parts_To_Make" sheetId="5" r:id="rId3"/>
+    <sheet name="Original_Multiphase" sheetId="1" r:id="rId4"/>
+    <sheet name="POL_Power_Breakdown" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,6 +38,265 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Windows PC</author>
+    <author>Shelby Riggleman</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{11F0AD10-D75E-4B26-8271-AC2DB1989F25}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+For 8 bit PWM Resolution, fPWM = ~280kHz</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB7" authorId="1" shapeId="0" xr:uid="{3FAF9296-22F1-433E-B148-CE8B5827756D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby Riggleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Resource here:
+https://www.cuidevices.com/blog/how-to-select-a-heat-sink</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{BBC868CC-B607-4691-B39F-3D63F2EBB6CC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows PC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note on operating in DCM vs CCM:https://electronics.stackexchange.com/questions/571412/how-does-the-inductor-current-ripple-influence-a-switch-mode-power-supply</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{AEEAC5CA-8DCF-4342-A9FB-E0D9E711CC13}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman: 50% comes from diminishing returns of shrinking inductor past ripple value &gt; 50% of avg current</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{1AB68726-C85B-4137-9733-5F2E29D05067}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby R:
+Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U8" authorId="0" shapeId="0" xr:uid="{65EB448B-9DF3-4C45-8EF5-36E7649E6C3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Capacitor Current Rating Must be higher than this value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{95AAF2F0-5BFB-49C5-9E05-5A369CB638BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby R:
+Alternative Part option:PA4349.104ANLT
+Wurth chosen because of AC loss simulator</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{7E98426D-287D-4E71-A451-CDAA1633D139}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+Chose as opposed to D2-Pak package due to chip shortage - 4200 available on Mouser and interchangable if necessary</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{86AFC510-9152-400C-A41A-E96187C1EBDE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+Excellent resource on gate charge characteristics: 
+https://www.microsemi.com/document-portal/doc_view/14697-making-use-of-gate-charge-information-in-mosfet-and-igbt-data-sheets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{6AA711BF-0F59-4FCE-A299-2D48672DAC94}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+The Total Gate Charge (Qg) is the amount of charge that needs to be injected into the gate electrode to turn ON (drive) the MOSFET.
+https://www.rohm.com/electronics-basics/transistors/total-gate-charge</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{12544BA5-11AB-4DB6-9097-3E530915C9C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+This is the charge that is relevant for switching losses = Qgd + (Qg-Qgd-Qgth)=Qsw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{0F6D26CA-EA06-47A4-BAE3-AA5584C06A17}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helpful page on benefits of low Qrr:
+https://efficiencywins.nexperia.com/efficient-products/qrr-overlooked-and-underappreciated-in-efficiency-battle.html</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB23" authorId="1" shapeId="0" xr:uid="{C3DC9D71-901E-4560-A9DD-3BDACE95F076}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby Riggleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rule of thumb is to assume thermal resistance of heat sink is actually 33% higher than posted due to point load nature of transistor connection, rather than heat being applied evenly across the heatsink</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{EEBC23EC-5FF1-493A-8ADD-A03FA5698FB3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S.Riggleman</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Taken from Wurth Loss calculator: https://redexpert.we-online.com/redexpert/#/module/7104/selecteditems/74437529203101/productdata/=74437529203101/type/+or+Single+Single_HV/Ir/gte:6A/Tris/lte:80K/Isat/gte:7.5A/applicationbar/LossCalculator/on/frequency/80kHz+0.5/inductorType/Single+Suitable/winding1/6A+DeltaIA+3A+2V+-2V
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows PC</author>
@@ -295,7 +555,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows PC</author>
@@ -320,7 +580,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows PC</author>
@@ -499,7 +759,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="172">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -994,6 +1254,27 @@
   </si>
   <si>
     <t>CCM vs DCM mode of operation advantages?</t>
+  </si>
+  <si>
+    <t>Rectifier Diode</t>
+  </si>
+  <si>
+    <t>STPS4S200S</t>
+  </si>
+  <si>
+    <t>Alt Part:</t>
+  </si>
+  <si>
+    <t>TSP10H200S S1G</t>
+  </si>
+  <si>
+    <t>Forward Voltage drop @ 6A</t>
+  </si>
+  <si>
+    <t>Avg Conduction Loss (per diode)</t>
+  </si>
+  <si>
+    <t>Total Conduction Loss:</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1112,22 +1393,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1913,11 +2197,956 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8223AA-8B6A-4046-920B-D31042179875}">
+  <dimension ref="A1:AC38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="41.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <f>SUM(K34,K32,K30,K28,H26,H24,N24,Y23,Q24)</f>
+        <v>19.423469424496901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4">
+        <f>((B19-H3)/B19)</f>
+        <v>0.97785136217786794</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>76000</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="J7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="14"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="S7" s="14"/>
+      <c r="U7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="V7" s="13"/>
+      <c r="X7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <f>E7/E9</f>
+        <v>76000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <f>E13*0.5</f>
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <f>SQRT(E10)*E13</f>
+        <v>4.2107006542854597</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="R8" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8">
+        <f>H20/SQRT(12)</f>
+        <v>0.91140057691430232</v>
+      </c>
+      <c r="U8" t="s">
+        <v>102</v>
+      </c>
+      <c r="V8">
+        <f>E14*SQRT(E10/(1-E10))</f>
+        <v>2.849679356962814</v>
+      </c>
+      <c r="X8" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>48.72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9">
+        <f>(B16*E10)/(H8*E8)</f>
+        <v>1.0523947368421052E-4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9">
+        <f>SQRT(1-E10)*E13</f>
+        <v>4.2743420546325028</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="X9" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y9">
+        <v>0.3</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC9">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <f>(B18-B16)/B18</f>
+        <v>0.49249999999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <f>(H8/2) + E13</f>
+        <v>7.5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" t="s">
+        <v>72</v>
+      </c>
+      <c r="X10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y10">
+        <v>12</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC10">
+        <f>AC9-AC8</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>0.95</v>
+      </c>
+      <c r="M11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC11">
+        <f>K26+K29+K31+K33</f>
+        <v>1.5978000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <f>E11*B19</f>
+        <v>833.11199999999997</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC12">
+        <f>AC10/AC11</f>
+        <v>50.068844661409436</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <f>(B17/B8)</f>
+        <v>6</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="J13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="M13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="14"/>
+      <c r="P13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="14"/>
+      <c r="U13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <f>(E12/B8)/B18</f>
+        <v>2.8927499999999999</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="7">
+        <v>74437529203101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q14">
+        <v>0.85</v>
+      </c>
+      <c r="R14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <f>100*POWER(10,-6)</f>
+        <v>9.9999999999999991E-5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="M15" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15">
+        <v>2E-3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>103</v>
+      </c>
+      <c r="V15">
+        <f>1000*POWER(10,-6)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC15">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f>B9</f>
+        <v>48.72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>2.29E-2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16">
+        <f>70*POWER(10,-9)</f>
+        <v>7.0000000000000005E-8</v>
+      </c>
+      <c r="U16" t="s">
+        <v>104</v>
+      </c>
+      <c r="V16">
+        <v>0.02</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC16">
+        <v>1.12E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f>B8*B10</f>
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17">
+        <v>9.4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17">
+        <f>56*POWER(10,-9)</f>
+        <v>5.6000000000000005E-8</v>
+      </c>
+      <c r="U17" t="s">
+        <v>107</v>
+      </c>
+      <c r="V17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC17">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>B13</f>
+        <v>96</v>
+      </c>
+      <c r="J18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18">
+        <f>179*POWER(10,-9)</f>
+        <v>1.79E-7</v>
+      </c>
+      <c r="U18" t="s">
+        <v>109</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC18">
+        <f>(AC17/AC16)*(1/AC15)</f>
+        <v>0.4520795660036166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <f>B16*B17</f>
+        <v>876.96</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19">
+        <f>478*POWER(10,-9)</f>
+        <v>4.7800000000000002E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <f>(B16*E10)/(H15*E8)</f>
+        <v>3.1571842105263159</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20">
+        <f>K17/N14</f>
+        <v>1.8666666666666668E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <f>E13+(0.5*H20)</f>
+        <v>7.5785921052631577</v>
+      </c>
+      <c r="J21" t="s">
+        <v>137</v>
+      </c>
+      <c r="K21">
+        <v>62</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
+        <v>6.0688261642264658</v>
+      </c>
+      <c r="J22" t="s">
+        <v>145</v>
+      </c>
+      <c r="K22">
+        <v>0.5</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="P22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="V22" s="13"/>
+      <c r="X22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y22" s="13"/>
+      <c r="AB22" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC22">
+        <f>AC12-AC18-K22</f>
+        <v>49.116765095405817</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23">
+        <f>POWER(H22,2)*H16</f>
+        <v>0.84342190816563356</v>
+      </c>
+      <c r="J23" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23">
+        <v>175</v>
+      </c>
+      <c r="M23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N23">
+        <f>B9*((E9*K16*E8) + N15)</f>
+        <v>0.35663040000000001</v>
+      </c>
+      <c r="P23" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q23">
+        <f>Q14*E14</f>
+        <v>2.4588375</v>
+      </c>
+      <c r="U23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V23">
+        <f>V18*V15</f>
+        <v>1E-3</v>
+      </c>
+      <c r="X23" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y23">
+        <f>Y10*Y9</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="AB23" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC23" s="13">
+        <f>AC22*0.666</f>
+        <v>32.711765553540275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24">
+        <f>H23*B8</f>
+        <v>2.5302657244969007</v>
+      </c>
+      <c r="M24" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24">
+        <f>N23*B8</f>
+        <v>1.0698912</v>
+      </c>
+      <c r="P24" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q24">
+        <f>Q23*B8</f>
+        <v>7.3765125000000005</v>
+      </c>
+      <c r="U24" t="s">
+        <v>106</v>
+      </c>
+      <c r="V24">
+        <f>V16/V18</f>
+        <v>0.02</v>
+      </c>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="13"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25">
+        <v>1.78E-2</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="U25" t="s">
+        <v>108</v>
+      </c>
+      <c r="V25">
+        <f>(H20*E10)/(E8*V23)</f>
+        <v>2.0459384522160663E-2</v>
+      </c>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="13"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26">
+        <f>H25*B8</f>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26">
+        <f>POWER(K8,2)*K15</f>
+        <v>0.12765599999999996</v>
+      </c>
+      <c r="U26" t="s">
+        <v>110</v>
+      </c>
+      <c r="V26">
+        <f>E14/(E9*(1-E10))</f>
+        <v>5.6999999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>111</v>
+      </c>
+      <c r="V27">
+        <f>V26*V16</f>
+        <v>0.11399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28">
+        <f>SUM(K26:K27)*B8</f>
+        <v>0.38296799999999986</v>
+      </c>
+      <c r="U28" t="s">
+        <v>112</v>
+      </c>
+      <c r="V28">
+        <f>SQRT(POWER(V25,2) + POWER(V27,2))</f>
+        <v>0.11582135560865113</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29">
+        <f>B18*E13*K20*E8</f>
+        <v>0.8171520000000001</v>
+      </c>
+      <c r="AB29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC29" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30">
+        <f>K29*B8</f>
+        <v>2.4514560000000003</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC30">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K31">
+        <f>(K18/2)*B18*E8</f>
+        <v>0.65299200000000002</v>
+      </c>
+      <c r="AB31" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC31">
+        <f>AC30*1.33</f>
+        <v>7.4479999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32">
+        <f>K31*B8</f>
+        <v>1.9589760000000001</v>
+      </c>
+      <c r="AB32" s="10"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34">
+        <f>K33*B8</f>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC35">
+        <f>AC11*(K22+AC18+AC31)+AC8</f>
+        <v>58.421647130560579</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="AB23:AB25"/>
+    <mergeCell ref="AC23:AC25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{F974E2C1-204C-46E0-AD74-524C67B91E81}"/>
+    <hyperlink ref="H14" r:id="rId2" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{B8A080CF-EAB1-4146-AA91-5C92DC2E8FF1}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{40C27283-5C28-44E9-9372-6CF38344C93F}"/>
+    <hyperlink ref="N9" r:id="rId4" xr:uid="{C9A154E1-D391-46E7-8389-0B97EB7C7B5D}"/>
+    <hyperlink ref="V14" r:id="rId5" xr:uid="{3ACF85BB-58A3-47A6-9A99-FBCE40ED275B}"/>
+    <hyperlink ref="AC29" r:id="rId6" xr:uid="{0D651D3E-BA1E-41E6-A218-8BFFE4AAAC62}"/>
+    <hyperlink ref="Q8" r:id="rId7" display="https://www.mouser.com/ProductDetail/STMicroelectronics/STPS4S200S?qs=BA62vJVifGo1urUInSDhRQ%3D%3D" xr:uid="{672D5FE1-9947-4353-AAF3-5C91194CF443}"/>
+    <hyperlink ref="Q9" r:id="rId8" xr:uid="{EE9A374B-AAAE-41B1-BBC4-AC8938AABF62}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1936,25 +3165,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1967,8 +3196,8 @@
         <v>67</v>
       </c>
       <c r="H3">
-        <f>SUM(K34,K32,K30,K28,H26,H24,N23,Y23)</f>
-        <v>25.043733816358454</v>
+        <f>SUM(K34,K32,K30,K28,H26,H24,N24,Y23)</f>
+        <v>24.863028924496902</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
@@ -1977,28 +3206,28 @@
       </c>
       <c r="H4">
         <f>((B19-H3)/B19)</f>
-        <v>0.97144255859291362</v>
+        <v>0.97164861689872184</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2008,31 +3237,31 @@
         <v>15</v>
       </c>
       <c r="E7">
-        <v>80000</v>
-      </c>
-      <c r="G7" s="13" t="s">
+        <v>76000</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="13"/>
+      <c r="J7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="13" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="13"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="13"/>
-      <c r="U7" s="13" t="s">
+      <c r="S7" s="14"/>
+      <c r="U7" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="14"/>
+      <c r="V7" s="13"/>
       <c r="X7" s="1" t="s">
         <v>132</v>
       </c>
@@ -2052,7 +3281,7 @@
       </c>
       <c r="E8">
         <f>E7/E9</f>
-        <v>80000</v>
+        <v>76000</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -2079,7 +3308,7 @@
       </c>
       <c r="S8">
         <f>H20/SQRT(12)</f>
-        <v>0.86583054806858728</v>
+        <v>0.91140057691430232</v>
       </c>
       <c r="U8" t="s">
         <v>102</v>
@@ -2119,7 +3348,7 @@
       </c>
       <c r="H9">
         <f>(B16*E10)/(H8*E8)</f>
-        <v>9.9977499999999989E-5</v>
+        <v>1.0523947368421052E-4</v>
       </c>
       <c r="J9" t="s">
         <v>45</v>
@@ -2206,7 +3435,7 @@
       </c>
       <c r="AC11">
         <f>K26+K29+K31+K33</f>
-        <v>5.3462160000000001</v>
+        <v>5.0852880000000003</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
@@ -2225,7 +3454,7 @@
       </c>
       <c r="AC12">
         <f>AC10/AC11</f>
-        <v>14.963854808709561</v>
+        <v>15.731655709568464</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
@@ -2242,26 +3471,26 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="H13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="M13" s="13" t="s">
+      <c r="K13" s="13"/>
+      <c r="M13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="13"/>
-      <c r="R13" s="13" t="s">
+      <c r="N13" s="14"/>
+      <c r="R13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="U13" s="13" t="s">
+      <c r="S13" s="14"/>
+      <c r="U13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="14"/>
+      <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -2444,10 +3673,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="14"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2462,7 +3691,7 @@
       </c>
       <c r="H20">
         <f>(B16*E10)/(H15*E8)</f>
-        <v>2.9993250000000002</v>
+        <v>3.1571842105263159</v>
       </c>
       <c r="J20" t="s">
         <v>58</v>
@@ -2478,7 +3707,7 @@
       </c>
       <c r="H21">
         <f>E13+(0.5*H20)</f>
-        <v>7.4996625000000003</v>
+        <v>7.5785921052631577</v>
       </c>
       <c r="J21" t="s">
         <v>137</v>
@@ -2496,7 +3725,7 @@
       </c>
       <c r="H22">
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
-        <v>6.0621499930279485</v>
+        <v>6.0688261642264658</v>
       </c>
       <c r="J22" t="s">
         <v>145</v>
@@ -2504,24 +3733,24 @@
       <c r="K22">
         <v>0.5</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="14"/>
-      <c r="U22" s="13" t="s">
+      <c r="N22" s="13"/>
+      <c r="U22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="V22" s="14"/>
-      <c r="X22" s="13" t="s">
+      <c r="V22" s="13"/>
+      <c r="X22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="Y22" s="14"/>
+      <c r="Y22" s="13"/>
       <c r="AB22" t="s">
         <v>151</v>
       </c>
       <c r="AC22">
         <f>AC12-AC18-K22</f>
-        <v>14.011775242705944</v>
+        <v>14.779576143564848</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2530,7 +3759,7 @@
       </c>
       <c r="H23">
         <f>POWER(H22,2)*H16</f>
-        <v>0.84156727211948457</v>
+        <v>0.84342190816563356</v>
       </c>
       <c r="J23" t="s">
         <v>141</v>
@@ -2543,7 +3772,7 @@
       </c>
       <c r="N23">
         <f>B9*((E9*K16*E8) + N15)</f>
-        <v>0.37027200000000005</v>
+        <v>0.35663040000000001</v>
       </c>
       <c r="U23" t="s">
         <v>105</v>
@@ -2559,12 +3788,12 @@
         <f>Y10*Y9</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="AB23" s="15" t="s">
+      <c r="AB23" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="AC23" s="14">
+      <c r="AC23" s="13">
         <f>AC22*0.666</f>
-        <v>9.3318423116421592</v>
+        <v>9.8431977116141898</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
@@ -2573,14 +3802,14 @@
       </c>
       <c r="H24">
         <f>H23*B8</f>
-        <v>2.5247018163584536</v>
+        <v>2.5302657244969007</v>
       </c>
       <c r="M24" t="s">
         <v>98</v>
       </c>
       <c r="N24">
         <f>N23*B8</f>
-        <v>1.1108160000000002</v>
+        <v>1.0698912</v>
       </c>
       <c r="U24" t="s">
         <v>106</v>
@@ -2589,8 +3818,8 @@
         <f>V16/V18</f>
         <v>0.02</v>
       </c>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="14"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G25" s="5" t="s">
@@ -2599,19 +3828,19 @@
       <c r="H25">
         <v>1.78E-2</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="14"/>
+      <c r="K25" s="13"/>
       <c r="U25" t="s">
         <v>108</v>
       </c>
       <c r="V25">
         <f>(H20*E10)/(E8*V23)</f>
-        <v>1.846459453125E-2</v>
-      </c>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="14"/>
+        <v>2.0459384522160663E-2</v>
+      </c>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="13"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="G26" s="5" t="s">
@@ -2665,7 +3894,7 @@
       </c>
       <c r="V28">
         <f>SQRT(POWER(V25,2) + POWER(V27,2))</f>
-        <v>0.11548567552386514</v>
+        <v>0.11582135560865113</v>
       </c>
       <c r="AB28" s="1" t="s">
         <v>26</v>
@@ -2677,7 +3906,7 @@
       </c>
       <c r="K29">
         <f>B18*E13*K20*E8</f>
-        <v>0.86016000000000015</v>
+        <v>0.8171520000000001</v>
       </c>
       <c r="AB29" s="5" t="s">
         <v>154</v>
@@ -2692,7 +3921,7 @@
       </c>
       <c r="K30">
         <f>K29*B8</f>
-        <v>2.5804800000000006</v>
+        <v>2.4514560000000003</v>
       </c>
       <c r="AB30" t="s">
         <v>156</v>
@@ -2707,7 +3936,7 @@
       </c>
       <c r="K31">
         <f>(K18/2)*B18*E8</f>
-        <v>0.68735999999999997</v>
+        <v>0.65299200000000002</v>
       </c>
       <c r="AB31" s="10" t="s">
         <v>158</v>
@@ -2723,7 +3952,7 @@
       </c>
       <c r="K32">
         <f>K31*2*B8</f>
-        <v>4.1241599999999998</v>
+        <v>3.9179520000000001</v>
       </c>
       <c r="AB32" s="10"/>
     </row>
@@ -2733,7 +3962,7 @@
       </c>
       <c r="K33">
         <f>K19*B18*E8</f>
-        <v>3.6710400000000005</v>
+        <v>3.4874880000000004</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
@@ -2742,7 +3971,7 @@
       </c>
       <c r="K34">
         <f>K33*B8</f>
-        <v>11.013120000000001</v>
+        <v>10.462464000000001</v>
       </c>
       <c r="AB34" s="1" t="s">
         <v>33</v>
@@ -2757,7 +3986,7 @@
       </c>
       <c r="AC35">
         <f>AC11*(K22+AC18+AC31)+AC8</f>
-        <v>89.908639777041586</v>
+        <v>87.716823816043387</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
@@ -2777,6 +4006,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
     <mergeCell ref="AB23:AB25"/>
     <mergeCell ref="AC23:AC25"/>
     <mergeCell ref="J25:K25"/>
@@ -2793,11 +4027,6 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -2813,7 +4042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81E0D2E-BF7B-44F8-984B-BF407D8DCAAB}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -2955,7 +4184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
   <dimension ref="A1:V31"/>
   <sheetViews>
@@ -2976,25 +4205,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3024,30 +4253,30 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -3059,26 +4288,26 @@
       <c r="E7">
         <v>450000</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="13"/>
+      <c r="J7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -3114,11 +4343,11 @@
       <c r="N8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -3153,11 +4382,11 @@
       <c r="N9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -3186,11 +4415,11 @@
       <c r="N10" t="s">
         <v>72</v>
       </c>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
@@ -3205,11 +4434,11 @@
       <c r="N11" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -3222,11 +4451,11 @@
         <f>E11*B19</f>
         <v>833.11199999999997</v>
       </c>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3242,23 +4471,23 @@
         <f>(B17/E9)</f>
         <v>9</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="H13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="M13" s="13" t="s">
+      <c r="K13" s="13"/>
+      <c r="M13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="13"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
+      <c r="N13" s="14"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -3286,11 +4515,11 @@
       <c r="N14">
         <v>3</v>
       </c>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -3315,11 +4544,11 @@
       <c r="N15">
         <v>2E-3</v>
       </c>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3342,11 +4571,11 @@
         <f>70*POWER(10,-9)</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -3394,10 +4623,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="14"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -3439,14 +4668,14 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="14"/>
-      <c r="M22" s="13" t="s">
+      <c r="K22" s="13"/>
+      <c r="M22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="13"/>
+      <c r="N22" s="14"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G23" s="5" t="s">
@@ -3572,6 +4801,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="R6:V16"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
@@ -3581,11 +4815,6 @@
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
@@ -3599,7 +4828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585350FB-4F44-44C9-BD54-CA099149966A}">
   <dimension ref="A1:K6"/>
   <sheetViews>

</xml_diff>

<commit_message>
work on pwm conditioning
</commit_message>
<xml_diff>
--- a/mppt/design/Converter_calculations.xlsx
+++ b/mppt/design/Converter_calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4841EE-0056-4E05-8580-36FCDA5FF8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B387E4B-B0A3-4E5B-8780-FFA5C2D6DABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -759,7 +759,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="173">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -1275,6 +1275,9 @@
   </si>
   <si>
     <t>Total Conduction Loss:</t>
+  </si>
+  <si>
+    <t>MIC4104YM</t>
   </si>
 </sst>
 </file>
@@ -1396,19 +1399,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2200,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8223AA-8B6A-4046-920B-D31042179875}">
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,25 +2225,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2296,29 +2299,29 @@
       <c r="E7">
         <v>76000</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="13"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="14"/>
+      <c r="N7" s="12"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14" t="s">
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="14"/>
-      <c r="U7" s="14" t="s">
+      <c r="S7" s="12"/>
+      <c r="U7" s="12" t="s">
         <v>101</v>
       </c>
       <c r="V7" s="13"/>
@@ -2473,7 +2476,7 @@
         <v>71</v>
       </c>
       <c r="N10" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="X10" t="s">
         <v>76</v>
@@ -2543,26 +2546,26 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="12"/>
+      <c r="J13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="14"/>
+      <c r="N13" s="12"/>
       <c r="P13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="14" t="s">
+      <c r="R13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="14"/>
-      <c r="U13" s="14" t="s">
+      <c r="S13" s="12"/>
+      <c r="U13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="V13" s="13"/>
@@ -2754,10 +2757,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="12"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2814,18 +2817,18 @@
       <c r="K22">
         <v>0.5</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="N22" s="13"/>
       <c r="P22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U22" s="14" t="s">
+      <c r="U22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="V22" s="13"/>
-      <c r="X22" s="14" t="s">
+      <c r="X22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="Y22" s="13"/>
@@ -2879,7 +2882,7 @@
         <f>Y10*Y9</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="AB23" s="12" t="s">
+      <c r="AB23" s="14" t="s">
         <v>153</v>
       </c>
       <c r="AC23" s="13">
@@ -2916,7 +2919,7 @@
         <f>V16/V18</f>
         <v>0.02</v>
       </c>
-      <c r="AB24" s="12"/>
+      <c r="AB24" s="14"/>
       <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
@@ -2926,7 +2929,7 @@
       <c r="H25">
         <v>1.78E-2</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="13"/>
@@ -2937,7 +2940,7 @@
         <f>(H20*E10)/(E8*V23)</f>
         <v>2.0459384522160663E-2</v>
       </c>
-      <c r="AB25" s="12"/>
+      <c r="AB25" s="14"/>
       <c r="AC25" s="13"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
@@ -3102,11 +3105,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="AB23:AB25"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="AC23:AC25"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="R7:S7"/>
@@ -3117,13 +3122,11 @@
     <mergeCell ref="R13:S13"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="AB23:AB25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{F974E2C1-204C-46E0-AD74-524C67B91E81}"/>
@@ -3165,25 +3168,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3239,26 +3242,26 @@
       <c r="E7">
         <v>76000</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="13"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="14"/>
+      <c r="N7" s="12"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="R7" s="14" t="s">
+      <c r="R7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="14"/>
-      <c r="U7" s="14" t="s">
+      <c r="S7" s="12"/>
+      <c r="U7" s="12" t="s">
         <v>101</v>
       </c>
       <c r="V7" s="13"/>
@@ -3471,23 +3474,23 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="12"/>
+      <c r="J13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="R13" s="14" t="s">
+      <c r="N13" s="12"/>
+      <c r="R13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="14"/>
-      <c r="U13" s="14" t="s">
+      <c r="S13" s="12"/>
+      <c r="U13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="V13" s="13"/>
@@ -3673,10 +3676,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="12"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -3733,15 +3736,15 @@
       <c r="K22">
         <v>0.5</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="N22" s="13"/>
-      <c r="U22" s="14" t="s">
+      <c r="U22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="V22" s="13"/>
-      <c r="X22" s="14" t="s">
+      <c r="X22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="Y22" s="13"/>
@@ -3788,7 +3791,7 @@
         <f>Y10*Y9</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="AB23" s="12" t="s">
+      <c r="AB23" s="14" t="s">
         <v>153</v>
       </c>
       <c r="AC23" s="13">
@@ -3818,7 +3821,7 @@
         <f>V16/V18</f>
         <v>0.02</v>
       </c>
-      <c r="AB24" s="12"/>
+      <c r="AB24" s="14"/>
       <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
@@ -3828,7 +3831,7 @@
       <c r="H25">
         <v>1.78E-2</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="13"/>
@@ -3839,7 +3842,7 @@
         <f>(H20*E10)/(E8*V23)</f>
         <v>2.0459384522160663E-2</v>
       </c>
-      <c r="AB25" s="12"/>
+      <c r="AB25" s="14"/>
       <c r="AC25" s="13"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
@@ -4006,11 +4009,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="AB23:AB25"/>
     <mergeCell ref="AC23:AC25"/>
     <mergeCell ref="J25:K25"/>
@@ -4027,6 +4025,11 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -4205,25 +4208,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4270,13 +4273,13 @@
       <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -4288,11 +4291,11 @@
       <c r="E7">
         <v>450000</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="13"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="13"/>
@@ -4303,11 +4306,11 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -4343,11 +4346,11 @@
       <c r="N8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -4382,11 +4385,11 @@
       <c r="N9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -4415,11 +4418,11 @@
       <c r="N10" t="s">
         <v>72</v>
       </c>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
@@ -4434,11 +4437,11 @@
       <c r="N11" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -4451,11 +4454,11 @@
         <f>E11*B19</f>
         <v>833.11199999999997</v>
       </c>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -4471,23 +4474,23 @@
         <f>(B17/E9)</f>
         <v>9</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="12"/>
+      <c r="J13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -4515,11 +4518,11 @@
       <c r="N14">
         <v>3</v>
       </c>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -4544,11 +4547,11 @@
       <c r="N15">
         <v>2E-3</v>
       </c>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -4571,11 +4574,11 @@
         <f>70*POWER(10,-9)</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -4623,10 +4626,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="12"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -4668,14 +4671,14 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="12" t="s">
         <v>33</v>
       </c>
       <c r="K22" s="13"/>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="14"/>
+      <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G23" s="5" t="s">
@@ -4801,11 +4804,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="R6:V16"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
@@ -4815,6 +4813,11 @@
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>

</xml_diff>